<commit_message>
cap nhat admin dashboard
</commit_message>
<xml_diff>
--- a/bang_luong.xlsx
+++ b/bang_luong.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,6 +530,37 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bùi Anh Dũng</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2025</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
local updates before pull
</commit_message>
<xml_diff>
--- a/bang_luong.xlsx
+++ b/bang_luong.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,6 +561,68 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bùi Anh Dũng</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2025</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Bùi Anh Dũng</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>11</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2025</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>